<commit_message>
Added ROI labels for motor/sensory regions + temporal lobe gyri
</commit_message>
<xml_diff>
--- a/LFPAnalysis/YBA_ROI_labelled_alie.xlsx
+++ b/LFPAnalysis/YBA_ROI_labelled_alie.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexandrafink/Documents/GraduateSchool/SaezLab/SWB/anat_recons/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexandrafink/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A81A5DEA-417E-3B4A-96B7-49A20A2B22CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{833B0EB1-B49E-AC46-A6E7-5BF6B0B9BC20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="24780" windowHeight="17660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="yba_roi" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4841" uniqueCount="1507">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4841" uniqueCount="1506">
   <si>
     <t>Index</t>
   </si>
@@ -4532,9 +4532,6 @@
   </si>
   <si>
     <t>ITG</t>
-  </si>
-  <si>
-    <t>STG</t>
   </si>
   <si>
     <t>premotor</t>
@@ -5383,8 +5380,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K691"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A398" zoomScale="115" workbookViewId="0">
-      <selection activeCell="F385" sqref="F385"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6076,7 +6073,7 @@
         <v>54</v>
       </c>
       <c r="F20" t="s">
-        <v>1504</v>
+        <v>1505</v>
       </c>
       <c r="G20" t="s">
         <v>55</v>
@@ -6111,7 +6108,7 @@
         <v>54</v>
       </c>
       <c r="F21" t="s">
-        <v>1504</v>
+        <v>1505</v>
       </c>
       <c r="G21" t="s">
         <v>57</v>
@@ -6146,7 +6143,7 @@
         <v>54</v>
       </c>
       <c r="F22" t="s">
-        <v>1504</v>
+        <v>1505</v>
       </c>
       <c r="G22" t="s">
         <v>59</v>
@@ -6181,7 +6178,7 @@
         <v>54</v>
       </c>
       <c r="F23" t="s">
-        <v>1504</v>
+        <v>1505</v>
       </c>
       <c r="G23" t="s">
         <v>61</v>
@@ -6216,7 +6213,7 @@
         <v>54</v>
       </c>
       <c r="F24" t="s">
-        <v>1504</v>
+        <v>1505</v>
       </c>
       <c r="G24" t="s">
         <v>63</v>
@@ -6251,7 +6248,7 @@
         <v>54</v>
       </c>
       <c r="F25" t="s">
-        <v>1504</v>
+        <v>1505</v>
       </c>
       <c r="G25" t="s">
         <v>65</v>
@@ -6286,7 +6283,7 @@
         <v>54</v>
       </c>
       <c r="F26" t="s">
-        <v>1504</v>
+        <v>1505</v>
       </c>
       <c r="G26" t="s">
         <v>67</v>
@@ -6321,7 +6318,7 @@
         <v>69</v>
       </c>
       <c r="F27" t="s">
-        <v>1506</v>
+        <v>1505</v>
       </c>
       <c r="G27" t="s">
         <v>70</v>
@@ -6356,7 +6353,7 @@
         <v>69</v>
       </c>
       <c r="F28" t="s">
-        <v>1506</v>
+        <v>1505</v>
       </c>
       <c r="G28" t="s">
         <v>72</v>
@@ -6391,7 +6388,7 @@
         <v>69</v>
       </c>
       <c r="F29" t="s">
-        <v>1506</v>
+        <v>1505</v>
       </c>
       <c r="G29" t="s">
         <v>74</v>
@@ -6426,7 +6423,7 @@
         <v>69</v>
       </c>
       <c r="F30" t="s">
-        <v>1506</v>
+        <v>1505</v>
       </c>
       <c r="G30" t="s">
         <v>76</v>
@@ -6461,7 +6458,7 @@
         <v>69</v>
       </c>
       <c r="F31" t="s">
-        <v>1506</v>
+        <v>1505</v>
       </c>
       <c r="G31" t="s">
         <v>78</v>
@@ -6496,7 +6493,7 @@
         <v>69</v>
       </c>
       <c r="F32" t="s">
-        <v>1506</v>
+        <v>1505</v>
       </c>
       <c r="G32" t="s">
         <v>80</v>
@@ -6531,7 +6528,7 @@
         <v>69</v>
       </c>
       <c r="F33" t="s">
-        <v>1506</v>
+        <v>1505</v>
       </c>
       <c r="G33" t="s">
         <v>82</v>
@@ -11921,7 +11918,7 @@
         <v>428</v>
       </c>
       <c r="F187" t="s">
-        <v>1505</v>
+        <v>1494</v>
       </c>
       <c r="G187" t="s">
         <v>429</v>
@@ -11956,7 +11953,7 @@
         <v>428</v>
       </c>
       <c r="F188" t="s">
-        <v>1505</v>
+        <v>1494</v>
       </c>
       <c r="G188" t="s">
         <v>431</v>
@@ -11991,7 +11988,7 @@
         <v>428</v>
       </c>
       <c r="F189" t="s">
-        <v>1505</v>
+        <v>1494</v>
       </c>
       <c r="G189" t="s">
         <v>433</v>
@@ -12026,7 +12023,7 @@
         <v>428</v>
       </c>
       <c r="F190" t="s">
-        <v>1505</v>
+        <v>1494</v>
       </c>
       <c r="G190" t="s">
         <v>435</v>
@@ -12061,7 +12058,7 @@
         <v>428</v>
       </c>
       <c r="F191" t="s">
-        <v>1505</v>
+        <v>1494</v>
       </c>
       <c r="G191" t="s">
         <v>437</v>
@@ -12096,7 +12093,7 @@
         <v>439</v>
       </c>
       <c r="F192" t="s">
-        <v>1505</v>
+        <v>1504</v>
       </c>
       <c r="G192" t="s">
         <v>440</v>
@@ -12131,7 +12128,7 @@
         <v>439</v>
       </c>
       <c r="F193" t="s">
-        <v>1505</v>
+        <v>1504</v>
       </c>
       <c r="G193" t="s">
         <v>442</v>
@@ -12166,7 +12163,7 @@
         <v>439</v>
       </c>
       <c r="F194" t="s">
-        <v>1505</v>
+        <v>1504</v>
       </c>
       <c r="G194" t="s">
         <v>444</v>
@@ -12201,7 +12198,7 @@
         <v>439</v>
       </c>
       <c r="F195" t="s">
-        <v>1505</v>
+        <v>1504</v>
       </c>
       <c r="G195" t="s">
         <v>446</v>
@@ -18151,7 +18148,7 @@
         <v>54</v>
       </c>
       <c r="F365" t="s">
-        <v>1504</v>
+        <v>1505</v>
       </c>
       <c r="G365" t="s">
         <v>832</v>
@@ -18186,7 +18183,7 @@
         <v>54</v>
       </c>
       <c r="F366" t="s">
-        <v>1504</v>
+        <v>1505</v>
       </c>
       <c r="G366" t="s">
         <v>834</v>
@@ -18221,7 +18218,7 @@
         <v>54</v>
       </c>
       <c r="F367" t="s">
-        <v>1504</v>
+        <v>1505</v>
       </c>
       <c r="G367" t="s">
         <v>836</v>
@@ -18256,7 +18253,7 @@
         <v>54</v>
       </c>
       <c r="F368" t="s">
-        <v>1504</v>
+        <v>1505</v>
       </c>
       <c r="G368" t="s">
         <v>838</v>
@@ -18291,7 +18288,7 @@
         <v>54</v>
       </c>
       <c r="F369" t="s">
-        <v>1504</v>
+        <v>1505</v>
       </c>
       <c r="G369" t="s">
         <v>840</v>
@@ -18326,7 +18323,7 @@
         <v>54</v>
       </c>
       <c r="F370" t="s">
-        <v>1504</v>
+        <v>1505</v>
       </c>
       <c r="G370" t="s">
         <v>842</v>
@@ -18361,7 +18358,7 @@
         <v>54</v>
       </c>
       <c r="F371" t="s">
-        <v>1504</v>
+        <v>1505</v>
       </c>
       <c r="G371" t="s">
         <v>844</v>
@@ -18396,7 +18393,7 @@
         <v>69</v>
       </c>
       <c r="F372" t="s">
-        <v>1506</v>
+        <v>1505</v>
       </c>
       <c r="G372" t="s">
         <v>846</v>
@@ -18431,7 +18428,7 @@
         <v>69</v>
       </c>
       <c r="F373" t="s">
-        <v>1506</v>
+        <v>1505</v>
       </c>
       <c r="G373" t="s">
         <v>848</v>
@@ -18466,7 +18463,7 @@
         <v>69</v>
       </c>
       <c r="F374" t="s">
-        <v>1506</v>
+        <v>1505</v>
       </c>
       <c r="G374" t="s">
         <v>850</v>
@@ -18501,7 +18498,7 @@
         <v>69</v>
       </c>
       <c r="F375" t="s">
-        <v>1506</v>
+        <v>1505</v>
       </c>
       <c r="G375" t="s">
         <v>852</v>
@@ -18536,7 +18533,7 @@
         <v>69</v>
       </c>
       <c r="F376" t="s">
-        <v>1506</v>
+        <v>1505</v>
       </c>
       <c r="G376" t="s">
         <v>854</v>
@@ -18571,7 +18568,7 @@
         <v>69</v>
       </c>
       <c r="F377" t="s">
-        <v>1506</v>
+        <v>1505</v>
       </c>
       <c r="G377" t="s">
         <v>856</v>
@@ -18606,7 +18603,7 @@
         <v>69</v>
       </c>
       <c r="F378" t="s">
-        <v>1506</v>
+        <v>1505</v>
       </c>
       <c r="G378" t="s">
         <v>858</v>
@@ -23996,7 +23993,7 @@
         <v>428</v>
       </c>
       <c r="F532" t="s">
-        <v>1505</v>
+        <v>1494</v>
       </c>
       <c r="G532" t="s">
         <v>1166</v>
@@ -24031,7 +24028,7 @@
         <v>428</v>
       </c>
       <c r="F533" t="s">
-        <v>1505</v>
+        <v>1494</v>
       </c>
       <c r="G533" t="s">
         <v>1168</v>
@@ -24066,7 +24063,7 @@
         <v>428</v>
       </c>
       <c r="F534" t="s">
-        <v>1505</v>
+        <v>1494</v>
       </c>
       <c r="G534" t="s">
         <v>1170</v>
@@ -24101,7 +24098,7 @@
         <v>428</v>
       </c>
       <c r="F535" t="s">
-        <v>1505</v>
+        <v>1494</v>
       </c>
       <c r="G535" t="s">
         <v>1172</v>
@@ -24136,7 +24133,7 @@
         <v>428</v>
       </c>
       <c r="F536" t="s">
-        <v>1505</v>
+        <v>1494</v>
       </c>
       <c r="G536" t="s">
         <v>1174</v>
@@ -24171,7 +24168,7 @@
         <v>439</v>
       </c>
       <c r="F537" t="s">
-        <v>1505</v>
+        <v>1504</v>
       </c>
       <c r="G537" t="s">
         <v>1176</v>
@@ -24206,7 +24203,7 @@
         <v>439</v>
       </c>
       <c r="F538" t="s">
-        <v>1505</v>
+        <v>1504</v>
       </c>
       <c r="G538" t="s">
         <v>1178</v>
@@ -24241,7 +24238,7 @@
         <v>439</v>
       </c>
       <c r="F539" t="s">
-        <v>1505</v>
+        <v>1504</v>
       </c>
       <c r="G539" t="s">
         <v>1180</v>
@@ -24276,7 +24273,7 @@
         <v>439</v>
       </c>
       <c r="F540" t="s">
-        <v>1505</v>
+        <v>1504</v>
       </c>
       <c r="G540" t="s">
         <v>1182</v>

</xml_diff>